<commit_message>
Experimented with theme overriding, first draft of day 1 program.
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10607689_polimi_it/Documents/Uni/BEST/TheWebDays/WebDays2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="11_F25DC773A252ABDACC10489F899C7A1E5BDE58F3" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{ECDE8F14-B18C-4AEE-A7E5-9664B6714D9B}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="11_F25DC773A252ABDACC10489F899C7A1E5BDE58F3" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{385AE2F2-5A18-497E-9BC3-BE431D802E58}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +142,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -359,6 +365,26 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -367,9 +393,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -392,6 +417,18 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,22 +453,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -454,6 +485,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1143001</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63638EC4-1B5D-483B-898B-AFCA749B47CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95251" y="1"/>
+          <a:ext cx="1047750" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -722,7 +808,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.5703125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -731,266 +817,271 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="27"/>
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>0.59375</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>0.625</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>0.65625</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <v>0.66666666666666596</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="4"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>0.687499999999999</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>0.69791666666666596</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="13"/>
       <c r="G14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>0.718749999999999</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>0.72916666666666596</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>0.73958333333333204</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <v>0.749999999999999</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>0.76041666666666596</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="29"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>0.77083333333333204</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="7">
         <v>0.781249999999999</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <v>0.79166666666666596</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="25"/>
     </row>
     <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="7">
         <v>0.80208333333333204</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="22"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="25"/>
     </row>
     <row r="25" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12">
+      <c r="A25" s="11">
         <v>0.812499999999999</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B5:B12"/>
     <mergeCell ref="C5:C12"/>
@@ -1002,11 +1093,9 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="D21:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>